<commit_message>
line changed for linestring
</commit_message>
<xml_diff>
--- a/fs/home/administrator/geo/Geo.xlsx
+++ b/fs/home/administrator/geo/Geo.xlsx
@@ -44,7 +44,7 @@
     <t>Line</t>
   </si>
   <si>
-    <t>line</t>
+    <t>linestring</t>
   </si>
   <si>
     <t>Polygon</t>
@@ -72,7 +72,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -119,24 +119,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
-      <sz val="10.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b/>
       <i val="0"/>
       <strike val="0"/>
@@ -191,6 +173,15 @@
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b val="0"/>
       <i val="0"/>
       <strike val="0"/>
@@ -209,7 +200,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,12 +253,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFEFEFEF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -291,26 +288,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -344,6 +321,19 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -356,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" fontId="0">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
@@ -364,26 +354,25 @@
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
     <xf applyBorder="1" fillId="3" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="2" applyFill="1"/>
-    <xf applyBorder="1" fillId="0" xfId="0" numFmtId="0" borderId="2" applyFont="1" fontId="3"/>
-    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="4">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" fillId="0" xfId="0" numFmtId="0" borderId="3" applyFont="1" fontId="5"/>
-    <xf applyBorder="1" fillId="4" xfId="0" numFmtId="0" borderId="4" applyFont="1" fontId="6" applyFill="1"/>
-    <xf applyAlignment="1" fillId="5" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="7" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="8"/>
-    <xf applyBorder="1" fillId="0" xfId="0" numFmtId="0" borderId="5" applyFont="1" fontId="9"/>
-    <xf applyBorder="1" fillId="6" xfId="0" numFmtId="0" borderId="6" applyFont="1" fontId="10" applyFill="1"/>
-    <xf applyAlignment="1" fillId="7" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="11" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" fillId="8" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="12" applyFill="1">
-      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
-    </xf>
-    <xf applyBorder="1" fillId="0" xfId="0" numFmtId="0" borderId="7" applyFont="1" fontId="13"/>
-    <xf applyAlignment="1" fillId="9" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="14" applyFill="1">
+    <xf applyAlignment="1" fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="3">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyBorder="1" fillId="4" xfId="0" numFmtId="0" borderId="2" applyFont="1" fontId="4" applyFill="1"/>
+    <xf applyAlignment="1" fillId="5" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="5" applyFill="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf fillId="0" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="6"/>
+    <xf applyBorder="1" fillId="0" xfId="0" numFmtId="0" borderId="3" applyFont="1" fontId="7"/>
+    <xf applyBorder="1" fillId="6" xfId="0" numFmtId="0" borderId="4" applyFont="1" fontId="8" applyFill="1"/>
+    <xf applyAlignment="1" fillId="7" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="9" applyFill="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" fillId="8" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="10" applyFill="1">
+      <alignment vertical="bottom" horizontal="general" wrapText="1"/>
+    </xf>
+    <xf applyBorder="1" fillId="9" xfId="0" numFmtId="0" borderId="5" applyFont="1" fontId="11" applyFill="1"/>
+    <xf applyBorder="1" fillId="0" xfId="0" numFmtId="0" borderId="6" applyFont="1" fontId="12"/>
+    <xf applyAlignment="1" fillId="10" xfId="0" numFmtId="0" borderId="0" applyFont="1" fontId="13" applyFill="1">
       <alignment vertical="bottom" horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -400,20 +389,20 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="10.0" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" customWidth="1" max="6" style="8" width="26.0"/>
+    <col min="1" customWidth="1" max="6" style="6" width="26.0"/>
   </cols>
   <sheetData>
-    <row customHeight="1" s="6" customFormat="1" r="1" ht="15.0">
-      <c t="s" s="2" r="A1">
+    <row customHeight="1" s="4" customFormat="1" r="1" ht="15.0">
+      <c t="s" s="11" r="A1">
         <v>0</v>
       </c>
-      <c t="s" s="2" r="B1">
+      <c t="s" s="11" r="B1">
         <v>1</v>
       </c>
-      <c t="s" s="2" r="C1">
+      <c t="s" s="11" r="C1">
         <v>2</v>
       </c>
-      <c t="s" s="2" r="D1">
+      <c t="s" s="11" r="D1">
         <v>3</v>
       </c>
       <c t="s" s="2" r="E1">
@@ -424,105 +413,105 @@
       </c>
     </row>
     <row r="2">
-      <c t="s" s="5" r="A2">
+      <c t="s" s="6" r="A2">
         <v>6</v>
       </c>
-      <c t="s" s="13" r="B2">
+      <c t="s" s="6" r="B2">
         <v>7</v>
       </c>
-      <c t="s" s="13" r="C2">
+      <c t="s" s="6" r="C2">
         <v>8</v>
       </c>
-      <c s="5" r="D2">
+      <c s="6" r="D2">
         <v>0</v>
       </c>
-      <c s="13" r="E2"/>
-      <c s="13" r="F2"/>
+      <c s="12" r="E2"/>
+      <c s="12" r="F2"/>
     </row>
     <row r="3">
-      <c t="s" s="5" r="A3">
+      <c t="s" s="6" r="A3">
         <v>6</v>
       </c>
-      <c t="s" s="8" r="B3">
+      <c t="s" s="6" r="B3">
         <v>9</v>
       </c>
-      <c t="s" s="8" r="C3">
+      <c t="s" s="6" r="C3">
         <v>10</v>
       </c>
-      <c s="5" r="D3">
+      <c s="6" r="D3">
         <v>0</v>
       </c>
-      <c s="8" r="E3"/>
-      <c s="8" r="F3"/>
+      <c s="6" r="E3"/>
+      <c s="6" r="F3"/>
     </row>
     <row r="4">
-      <c t="s" s="5" r="A4">
+      <c t="s" s="6" r="A4">
         <v>6</v>
       </c>
-      <c t="s" s="3" r="B4">
+      <c t="s" s="6" r="B4">
         <v>11</v>
       </c>
-      <c t="s" s="3" r="C4">
+      <c t="s" s="6" r="C4">
         <v>12</v>
       </c>
-      <c s="13" r="D4">
+      <c s="6" r="D4">
         <v>0</v>
       </c>
-      <c s="8" r="E4"/>
-      <c s="8" r="F4"/>
+      <c s="6" r="E4"/>
+      <c s="6" r="F4"/>
     </row>
     <row r="5">
-      <c t="s" s="5" r="A5">
+      <c t="s" s="6" r="A5">
         <v>6</v>
       </c>
-      <c t="s" s="13" r="B5">
+      <c t="s" s="6" r="B5">
         <v>13</v>
       </c>
-      <c t="s" s="13" r="C5">
+      <c t="s" s="6" r="C5">
         <v>8</v>
       </c>
-      <c s="8" r="D5">
+      <c s="6" r="D5">
         <v>1</v>
       </c>
-      <c s="8" r="E5"/>
-      <c s="8" r="F5"/>
+      <c s="6" r="E5"/>
+      <c s="6" r="F5"/>
     </row>
     <row r="6">
-      <c t="s" s="5" r="A6">
+      <c t="s" s="6" r="A6">
         <v>6</v>
       </c>
-      <c t="s" s="8" r="B6">
+      <c t="s" s="6" r="B6">
         <v>14</v>
       </c>
-      <c t="s" s="8" r="C6">
+      <c t="s" s="6" r="C6">
         <v>10</v>
       </c>
-      <c s="8" r="D6">
+      <c s="6" r="D6">
         <v>1</v>
       </c>
-      <c s="8" r="E6"/>
-      <c s="8" r="F6"/>
+      <c s="6" r="E6"/>
+      <c s="6" r="F6"/>
     </row>
     <row r="7">
-      <c t="s" s="13" r="A7">
+      <c t="s" s="6" r="A7">
         <v>6</v>
       </c>
-      <c t="s" s="8" r="B7">
+      <c t="s" s="6" r="B7">
         <v>15</v>
       </c>
-      <c t="s" s="8" r="C7">
+      <c t="s" s="6" r="C7">
         <v>12</v>
       </c>
-      <c s="8" r="D7">
+      <c s="6" r="D7">
         <v>1</v>
       </c>
-      <c s="8" r="E7"/>
-      <c s="8" r="F7"/>
+      <c s="6" r="E7"/>
+      <c s="6" r="F7"/>
     </row>
   </sheetData>
   <dataValidations>
     <dataValidation errorStyle="warning" showErrorMessage="1" sqref="C2:C7" allowBlank="1" type="list">
-      <formula1>"text,integer,decimal,binary,boolean,locale,date,datetime,point,line,polygon,"</formula1>
+      <formula1>"text,integer,decimal,binary,boolean,locale,date,datetime,point,linestring,polygon,"</formula1>
     </dataValidation>
   </dataValidations>
 </worksheet>
@@ -540,7 +529,7 @@
     <col min="5" customWidth="1" max="5" width="26.0"/>
   </cols>
   <sheetData>
-    <row customHeight="1" s="6" customFormat="1" r="1" ht="15.0">
+    <row customHeight="1" s="4" customFormat="1" r="1" ht="15.0">
       <c t="s" s="2" r="A1">
         <v>0</v>
       </c>

</xml_diff>